<commit_message>
Runs end to end without feasible solutions
</commit_message>
<xml_diff>
--- a/data/espn_rugby_data.xlsx
+++ b/data/espn_rugby_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurapallett/Desktop/fantasy_rugby/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurapallett/Documents/espn_fantasy_rugby/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C672288F-6DA2-3D4E-A501-31BE398BDE25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA0508-E93C-1645-850E-FA38C3C4F9C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16140" xr2:uid="{F4E93FC6-B9F6-D143-A36F-47FE27FE8D7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4730" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4730" uniqueCount="270">
   <si>
     <t>O Farrell</t>
   </si>
@@ -834,6 +834,18 @@
   <si>
     <t>ROUND</t>
   </si>
+  <si>
+    <t>P OMahony</t>
+  </si>
+  <si>
+    <t>L Cowan Dickie</t>
+  </si>
+  <si>
+    <t>B Teo</t>
+  </si>
+  <si>
+    <t>Z Fagerson</t>
+  </si>
 </sst>
 </file>
 
@@ -1223,12 +1235,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F97981-5D51-8D49-B1FC-CA5460516FF6}">
   <dimension ref="A1:W232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J206" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2:W232"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4429,7 +4442,7 @@
     </row>
     <row r="46" spans="1:23" ht="17">
       <c r="A46" s="3" t="s">
-        <v>81</v>
+        <v>266</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>17</v>
@@ -9044,7 +9057,7 @@
     </row>
     <row r="111" spans="1:23" ht="17">
       <c r="A111" s="3" t="s">
-        <v>158</v>
+        <v>267</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>1</v>
@@ -11032,7 +11045,7 @@
     </row>
     <row r="139" spans="1:23" ht="17">
       <c r="A139" s="3" t="s">
-        <v>194</v>
+        <v>268</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>1</v>
@@ -16357,7 +16370,7 @@
     </row>
     <row r="214" spans="1:23" ht="17">
       <c r="A214" s="3" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>4</v>

</xml_diff>